<commit_message>
added raw accuracy and nan
</commit_message>
<xml_diff>
--- a/tables/banknote_1.xlsx
+++ b/tables/banknote_1.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,86 +476,86 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr"/>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr"/>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>BAARD2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>BAARD3</t>
         </is>
       </c>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>FS</t>
         </is>
       </c>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>LID</t>
         </is>
       </c>
-      <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>RC</t>
         </is>
       </c>
-      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="B2" s="1" t="inlineStr"/>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr"/>
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>FPR</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Success</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>FPR</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>Success</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>FPR</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>Success</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>FPR</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>Success</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>FPR</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>Success</t>
         </is>
@@ -572,6 +572,11 @@
           <t>Epsilon</t>
         </is>
       </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy after attack</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -582,34 +587,37 @@
       <c r="B4" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="1" t="n">
+        <v>78.57142857142857</v>
+      </c>
+      <c r="D4" t="n">
         <v>6.122448979591836</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>97.44897959183672</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>8.163265306122449</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>99.48979591836736</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>48.97959183673469</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>87.24489795918367</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>1.530612244897959</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>92.85714285714286</v>
       </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
       <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>83.16326530612244</v>
       </c>
     </row>
@@ -618,34 +626,37 @@
       <c r="B5" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="1" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="D5" t="n">
         <v>6.122448979591836</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>99.48979591836736</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>8.163265306122449</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>99.48979591836736</v>
-      </c>
-      <c r="G5" t="n">
-        <v>51.53061224489795</v>
       </c>
       <c r="H5" t="n">
         <v>51.53061224489795</v>
       </c>
       <c r="I5" t="n">
+        <v>51.53061224489795</v>
+      </c>
+      <c r="J5" t="n">
         <v>1.020408163265306</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>72.44897959183673</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
       <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>52.55102040816326</v>
       </c>
     </row>
@@ -654,34 +665,37 @@
       <c r="B6" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="C6" t="n">
-        <v>2.551020408163265</v>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E6" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
         <v>39.28571428571428</v>
       </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
       <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
         <v>98.9795918367347</v>
       </c>
-      <c r="K6" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L6" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M6" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -690,34 +704,37 @@
       <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>2.551020408163265</v>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E7" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>40.81632653061224</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
       <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
         <v>93.36734693877553</v>
       </c>
-      <c r="K7" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L7" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M7" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -730,34 +747,37 @@
       <c r="B8" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="C8" t="n">
-        <v>2.551020408163265</v>
+      <c r="C8" s="1" t="n">
+        <v>63.77551020408163</v>
       </c>
       <c r="D8" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E8" t="n">
         <v>94.89795918367348</v>
       </c>
-      <c r="E8" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F8" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G8" t="n">
         <v>96.93877551020408</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>37.24489795918368</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>77.55102040816327</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>5.612244897959184</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>87.24489795918367</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L8" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M8" t="n">
         <v>72.44897959183673</v>
       </c>
     </row>
@@ -766,34 +786,37 @@
       <c r="B9" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="C9" t="n">
-        <v>2.551020408163265</v>
+      <c r="C9" s="1" t="n">
+        <v>5.102040816326531</v>
       </c>
       <c r="D9" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E9" t="n">
         <v>69.38775510204081</v>
       </c>
-      <c r="E9" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F9" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G9" t="n">
         <v>70.91836734693877</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
       <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
         <v>5.102040816326531</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>7.653061224489796</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>24.48979591836735</v>
       </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
       <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>56.12244897959183</v>
       </c>
     </row>
@@ -802,34 +825,37 @@
       <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" t="n">
-        <v>2.551020408163265</v>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E10" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F10" t="n">
-        <v>100</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>38.77551020408163</v>
       </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
       <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
         <v>98.46938775510203</v>
       </c>
-      <c r="K10" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L10" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M10" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -838,30 +864,33 @@
       <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C11" t="n">
-        <v>2.551020408163265</v>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E11" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F11" t="n">
-        <v>100</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -870,30 +899,33 @@
       <c r="B12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C12" t="n">
-        <v>2.551020408163265</v>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E12" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G12" t="n">
+        <v>100</v>
+      </c>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
         <v>97.95918367346938</v>
       </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
       <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -906,34 +938,37 @@
       <c r="B13" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="C13" t="n">
-        <v>2.551020408163265</v>
+      <c r="C13" s="1" t="n">
+        <v>9.183673469387756</v>
       </c>
       <c r="D13" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E13" t="n">
         <v>73.9795918367347</v>
       </c>
-      <c r="E13" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F13" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G13" t="n">
         <v>74.48979591836735</v>
       </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
       <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
         <v>9.183673469387756</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>6.63265306122449</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>39.28571428571428</v>
       </c>
-      <c r="K13" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L13" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M13" t="n">
         <v>57.6530612244898</v>
       </c>
     </row>
@@ -942,34 +977,37 @@
       <c r="B14" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="C14" t="n">
-        <v>2.551020408163265</v>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D14" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E14" t="n">
         <v>97.95918367346938</v>
       </c>
-      <c r="E14" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F14" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G14" t="n">
         <v>97.95918367346938</v>
       </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
         <v>1.020408163265306</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>91.32653061224489</v>
       </c>
-      <c r="K14" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L14" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M14" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -978,34 +1016,37 @@
       <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C15" t="n">
-        <v>2.551020408163265</v>
+      <c r="C15" s="1" t="n">
+        <v>0.5102040816326531</v>
       </c>
       <c r="D15" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E15" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F15" t="n">
-        <v>100</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
         <v>41.3265306122449</v>
       </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
       <c r="J15" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.5102040816326531</v>
+        <v>100</v>
       </c>
       <c r="L15" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M15" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -1014,30 +1055,33 @@
       <c r="B16" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C16" t="n">
-        <v>2.551020408163265</v>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E16" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F16" t="n">
-        <v>100</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G16" t="n">
+        <v>100</v>
+      </c>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
         <v>96.93877551020408</v>
       </c>
-      <c r="K16" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L16" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M16" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -1046,30 +1090,33 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" t="n">
-        <v>2.551020408163265</v>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E17" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F17" t="n">
-        <v>100</v>
-      </c>
-      <c r="G17" t="inlineStr"/>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100</v>
+      </c>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.5102040816326531</v>
+        <v>100</v>
       </c>
       <c r="L17" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M17" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -1082,34 +1129,37 @@
       <c r="B18" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="C18" t="n">
-        <v>2.551020408163265</v>
+      <c r="C18" s="1" t="n">
+        <v>52.04081632653062</v>
       </c>
       <c r="D18" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E18" t="n">
         <v>94.89795918367348</v>
       </c>
-      <c r="E18" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F18" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G18" t="n">
         <v>97.95918367346938</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>33.6734693877551</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>67.3469387755102</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>5.612244897959184</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>75.51020408163265</v>
       </c>
-      <c r="K18" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L18" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M18" t="n">
         <v>70.40816326530613</v>
       </c>
     </row>
@@ -1122,34 +1172,37 @@
       <c r="B19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C19" t="n">
-        <v>2.551020408163265</v>
+      <c r="C19" s="1" t="n">
+        <v>1.020408163265306</v>
       </c>
       <c r="D19" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E19" t="n">
         <v>86.73469387755102</v>
       </c>
-      <c r="E19" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F19" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G19" t="n">
         <v>95.91836734693877</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>47.44897959183674</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>34.18367346938776</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>5.102040816326531</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>56.63265306122449</v>
       </c>
-      <c r="K19" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L19" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M19" t="n">
         <v>35.20408163265306</v>
       </c>
     </row>
@@ -1158,34 +1211,37 @@
       <c r="B20" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C20" t="n">
-        <v>2.551020408163265</v>
+      <c r="C20" s="1" t="n">
+        <v>1.020408163265306</v>
       </c>
       <c r="D20" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E20" t="n">
         <v>67.3469387755102</v>
       </c>
-      <c r="E20" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F20" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G20" t="n">
         <v>67.3469387755102</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>47.44897959183674</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>52.04081632653062</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>9.693877551020408</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>34.18367346938776</v>
       </c>
-      <c r="K20" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L20" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M20" t="n">
         <v>59.69387755102041</v>
       </c>
     </row>
@@ -1194,34 +1250,37 @@
       <c r="B21" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C21" t="n">
-        <v>2.551020408163265</v>
+      <c r="C21" s="1" t="n">
+        <v>1.020408163265306</v>
       </c>
       <c r="D21" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E21" t="n">
         <v>91.32653061224489</v>
       </c>
-      <c r="E21" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F21" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G21" t="n">
         <v>91.32653061224489</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>46.42857142857143</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>51.02040816326531</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>1.020408163265306</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>79.59183673469387</v>
       </c>
-      <c r="K21" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L21" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M21" t="n">
         <v>59.69387755102041</v>
       </c>
     </row>
@@ -1234,34 +1293,37 @@
       <c r="B22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C22" t="n">
-        <v>2.551020408163265</v>
+      <c r="C22" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D22" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E22" t="n">
         <v>77.55102040816327</v>
       </c>
-      <c r="E22" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F22" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G22" t="n">
         <v>79.08163265306123</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>39.28571428571428</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>37.24489795918368</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>7.653061224489796</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>46.42857142857143</v>
       </c>
-      <c r="K22" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L22" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M22" t="n">
         <v>53.57142857142857</v>
       </c>
     </row>
@@ -1270,34 +1332,37 @@
       <c r="B23" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C23" t="n">
-        <v>2.551020408163265</v>
+      <c r="C23" s="1" t="n">
+        <v>1.020408163265306</v>
       </c>
       <c r="D23" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E23" t="n">
         <v>69.89795918367348</v>
       </c>
-      <c r="E23" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F23" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G23" t="n">
         <v>69.89795918367348</v>
-      </c>
-      <c r="G23" t="n">
-        <v>48.97959183673469</v>
       </c>
       <c r="H23" t="n">
         <v>48.97959183673469</v>
       </c>
       <c r="I23" t="n">
-        <v>4.591836734693878</v>
+        <v>48.97959183673469</v>
       </c>
       <c r="J23" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="K23" t="n">
         <v>52.55102040816326</v>
       </c>
-      <c r="K23" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L23" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M23" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -1310,34 +1375,37 @@
       <c r="B24" s="1" t="n">
         <v>1e-06</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="1" t="n">
+        <v>1.530612244897959</v>
+      </c>
+      <c r="D24" t="n">
         <v>6.122448979591836</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>95.91836734693877</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>8.163265306122449</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>96.93877551020408</v>
       </c>
-      <c r="G24" t="n">
-        <v>0</v>
-      </c>
       <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
         <v>33.6734693877551</v>
       </c>
-      <c r="I24" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="J24" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="K24" t="n">
         <v>87.75510204081633</v>
       </c>
-      <c r="K24" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L24" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M24" t="n">
         <v>54.59183673469388</v>
       </c>
     </row>
@@ -1350,34 +1418,37 @@
       <c r="B25" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="C25" t="n">
-        <v>2.551020408163265</v>
+      <c r="C25" s="1" t="n">
+        <v>76.0204081632653</v>
       </c>
       <c r="D25" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E25" t="n">
         <v>97.44897959183672</v>
       </c>
-      <c r="E25" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F25" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G25" t="n">
         <v>98.9795918367347</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>48.46938775510204</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>86.73469387755102</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>5.102040816326531</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>92.3469387755102</v>
       </c>
-      <c r="K25" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L25" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M25" t="n">
         <v>80.10204081632652</v>
       </c>
     </row>
@@ -1386,34 +1457,37 @@
       <c r="B26" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="C26" t="n">
-        <v>2.551020408163265</v>
+      <c r="C26" s="1" t="n">
+        <v>1.020408163265306</v>
       </c>
       <c r="D26" t="n">
+        <v>2.551020408163265</v>
+      </c>
+      <c r="E26" t="n">
         <v>98.46938775510203</v>
       </c>
-      <c r="E26" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="F26" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="G26" t="n">
         <v>98.46938775510203</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>47.95918367346938</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>53.06122448979592</v>
       </c>
-      <c r="I26" t="n">
-        <v>4.591836734693878</v>
-      </c>
       <c r="J26" t="n">
+        <v>4.591836734693878</v>
+      </c>
+      <c r="K26" t="n">
         <v>78.57142857142857</v>
       </c>
-      <c r="K26" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L26" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M26" t="n">
         <v>58.67346938775511</v>
       </c>
     </row>
@@ -1422,34 +1496,37 @@
       <c r="B27" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="C27" t="n">
-        <v>2.551020408163265</v>
+      <c r="C27" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E27" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F27" t="n">
-        <v>100</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
         <v>39.28571428571428</v>
       </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
       <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
         <v>98.46938775510203</v>
       </c>
-      <c r="K27" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L27" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M27" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
@@ -1458,44 +1535,47 @@
       <c r="B28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C28" t="n">
-        <v>2.551020408163265</v>
+      <c r="C28" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>100</v>
+        <v>2.551020408163265</v>
       </c>
       <c r="E28" t="n">
-        <v>4.591836734693878</v>
+        <v>100</v>
       </c>
       <c r="F28" t="n">
-        <v>100</v>
+        <v>4.591836734693878</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
         <v>40.81632653061224</v>
       </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
       <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
         <v>97.44897959183672</v>
       </c>
-      <c r="K28" t="n">
-        <v>0.5102040816326531</v>
-      </c>
       <c r="L28" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="M28" t="n">
         <v>59.18367346938776</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A17"/>

</xml_diff>